<commit_message>
Analyse: Welche Aspekte wollen wir für die Routenschnittstelle im Detail beleuchtet? [SPIKE] #14
</commit_message>
<xml_diff>
--- a/Research/AspektVergleich.xlsx
+++ b/Research/AspektVergleich.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwolpers\Bachelorarbeit\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Bachelorarbeit\GraphQL-\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589CE161-309C-485E-AD28-9D0A4DCF3CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1AE253-1709-4A04-9DC6-CF70998A7A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="7980" xr2:uid="{65CEA5B8-29B4-4704-9E67-E1B48F49D86F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65CEA5B8-29B4-4704-9E67-E1B48F49D86F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html;</t>
   </si>
   <si>
-    <t>REST, vor allem bei kleinen Projekten, wo die Entwickler noch keine Erfahrung mit GraphQL haben</t>
-  </si>
-  <si>
     <t>Hochladen von Daten?</t>
   </si>
   <si>
@@ -120,15 +117,6 @@
     <t>https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html; https://medium.com/paypal-engineering/scaling-graphql-at-paypal-b5b5ac098810</t>
   </si>
   <si>
-    <t>Dauer einen Lauffähigen Prototypen zu schreiben</t>
-  </si>
-  <si>
-    <t>Schnell und einfach</t>
-  </si>
-  <si>
-    <t>Aufwändig</t>
-  </si>
-  <si>
     <t>n+1 problematik</t>
   </si>
   <si>
@@ -142,6 +130,18 @@
   </si>
   <si>
     <t>auch verschiedene Endpunkte, macht es aber auch einfacher, Versionierung komplett zu vermeiden, möglichkeit gena zu erkennen welche felder benötigt werden</t>
+  </si>
+  <si>
+    <t>Streaming</t>
+  </si>
+  <si>
+    <t>Automatische Dokumentation?</t>
+  </si>
+  <si>
+    <t>Underfetching muss auch getestet werden</t>
+  </si>
+  <si>
+    <t>Paginierung</t>
   </si>
 </sst>
 </file>
@@ -518,18 +518,19 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="3" width="60.7109375" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" customWidth="1"/>
-    <col min="5" max="5" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="3" width="60.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.44140625" customWidth="1"/>
+    <col min="5" max="5" width="75.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -545,193 +546,193 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -739,7 +740,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -747,7 +748,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -755,7 +756,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -763,7 +764,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -771,7 +772,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -779,7 +780,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -787,7 +788,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -795,7 +796,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -803,7 +804,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -811,7 +812,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -819,7 +820,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -829,14 +830,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{A1E610CB-1F74-4E4A-9700-4FB6CCBC2B53}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{AACA2E41-80F1-4879-A331-3118E519859E}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{FBE89555-8532-4244-B465-91788320B8B6}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{626DC3E6-78AA-4010-BA55-77D33F0634BB}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{3918E471-D9F1-4828-B544-C0243E088B83}"/>
-    <hyperlink ref="E9" r:id="rId6" display="https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html;" xr:uid="{40F0907E-A9B5-4645-A630-444D03B702DD}"/>
-    <hyperlink ref="E10" r:id="rId7" display="https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html;" xr:uid="{7BE63C27-D55D-4582-8408-515D2E7DF3AE}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{FF1B2000-99D8-44AB-8A93-14EF25B795CC}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{A1E610CB-1F74-4E4A-9700-4FB6CCBC2B53}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{AACA2E41-80F1-4879-A331-3118E519859E}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{626DC3E6-78AA-4010-BA55-77D33F0634BB}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{3918E471-D9F1-4828-B544-C0243E088B83}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html;" xr:uid="{40F0907E-A9B5-4645-A630-444D03B702DD}"/>
+    <hyperlink ref="E11" r:id="rId6" display="https://www.dev-insider.de/graphql-als-alternative-zu-rest-a-752074/index2.html;" xr:uid="{7BE63C27-D55D-4582-8408-515D2E7DF3AE}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{FF1B2000-99D8-44AB-8A93-14EF25B795CC}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{FBE89555-8532-4244-B465-91788320B8B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>